<commit_message>
Initial Streamlit FAQ app with categories, search & styling
</commit_message>
<xml_diff>
--- a/faq.xlsx
+++ b/faq.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vee38533\source\repos\Docker\sesro-dt-faq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8804694D-16EE-4646-818D-B0231B3E6FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B847C6-4D4A-4848-83C1-88B1E26E8648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{0932D0B0-4534-4EDF-81FA-F2FD4759D06A}"/>
+    <workbookView xWindow="30870" yWindow="405" windowWidth="24915" windowHeight="13185" xr2:uid="{0932D0B0-4534-4EDF-81FA-F2FD4759D06A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,47 +411,6 @@
 5. Better Environmental Outcomes: A robust Impact Assessment, and a transparent, inclusive and thorough consultation plan will help derisk the SESRO project from a planning perspective, by reducing the probability of objections. This can increase the likelihood of consent being attained with minimal unplanned issues.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">In the context of the SESRO project, the Digital Twin comprises several components that together form a virtual representation of the physical infrastructure. These components include: 1. Foundation Data Model: This is a key enabler for the development of the Digital Twin. It provides a structured format for data, which ensures consistency and interoperability. Federated Model Environment: This component of the Common Data Environment (CDE) is crucial for maintaining an accurate digital replica of the physical asset during the delivery stage </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF123BB6"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF1C1C1C"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">. 3. Federated Data Platform: Another key enabler for the development of the Digital Twin, the Federated Data Platform facilitates the integration and management of data from various sources </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF123BB6"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF1C1C1C"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>. 4. Integration with Operational Technology (OT): Once the OT strategy is implemented, it will provide the necessary link between the physical and digital states of the SESRO infrastructure. Standards, methods, and procedures: These are established and enforced to ensure that an accurate digital replica of the physical asset is maintained in the CDE during the delivery stage. Compliance with SRO Information Management (IM) Requirements: The SESRO project will comply with the SRO Information Management (IM) Requirements Schedule to support the development of the Digital Twin.</t>
-    </r>
-  </si>
-  <si>
     <t>The Digital Twin for the SESRO project is developed from various data sources:
 1. Project Datasets: Project datasets are created and stored in the SESRO project's Spatial Data Environment (SDE) databases. The databases are hosted on Microsoft Azure and managed by Arup's Digital Technology Group.
 2. Reference Datasets: The Reference (REF) database contains any reference datasets collected for use on the project. No edits should be made to any datasets stored in this database.
@@ -552,6 +511,35 @@
   </si>
   <si>
     <t>Support &amp; Next Steps</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In the context of the SESRO project, the Digital Twin comprises several components that together form a virtual representation of the physical infrastructure. These components include: 
+1. Foundation Data Model: This is a key enabler for the development of the Digital Twin. It provides a structured format for data, which ensures consistency and interoperability. 
+2. Federated Model Environment: This component of the Common Data Environment (CDE) is crucial for maintaining an accurate digital replica of the physical asset during the delivery stage </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF123BB6"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF1C1C1C"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>. 
+3. Federated Data Platform: Another key enabler for the development of the Digital Twin, the Federated Data Platform facilitates the integration and management of data from various sources  
+4. Integration with Operational Technology (OT): Once the OT strategy is implemented, it will provide the necessary link between the physical and digital states of the SESRO infrastructure. 
+5.Standards, methods, and procedures: These are established and enforced to ensure that an accurate digital replica of the physical asset is maintained in the CDE during the delivery stage. Compliance with SRO Information Management (IM) Requirements: 
+The SESRO project will comply with the SRO Information Management (IM) Requirements Schedule to support the development of the Digital Twin.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -630,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -663,32 +651,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF123BB6"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -774,6 +741,25 @@
         <shadow val="0"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF123BB6"/>
         <name val="Segoe UI"/>
         <family val="2"/>
         <scheme val="none"/>
@@ -843,13 +829,13 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6D51F066-0A79-462B-97A8-DAD41F6D38A6}" name="Question" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{F6DC4E80-826A-4A3D-BA51-6C2CC268D059}" name="Answer" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{C1F402BA-0067-45B8-92F1-701892D6363E}" name="Category" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{C12F3253-365B-41BD-8015-F310FF9F1408}" name="Other Answer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{F0BAAB17-C885-4EAB-B097-C5640D8D6EE2}" name="Reference" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{DB3865D4-019A-4839-8130-32656724A830}" name="Column1" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{BEB02E25-0562-4C2D-B657-B538B8EE4A66}" name="Column2" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{DB85D41E-8FB1-4789-A3EA-B4AE5BBCD495}" name="Column3" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{7C801207-5395-41CC-B54D-9663C1FE511F}" name="Column4" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{C1F402BA-0067-45B8-92F1-701892D6363E}" name="Category" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C12F3253-365B-41BD-8015-F310FF9F1408}" name="Other Answer" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{F0BAAB17-C885-4EAB-B097-C5640D8D6EE2}" name="Reference" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{DB3865D4-019A-4839-8130-32656724A830}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{BEB02E25-0562-4C2D-B657-B538B8EE4A66}" name="Column2" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{DB85D41E-8FB1-4789-A3EA-B4AE5BBCD495}" name="Column3" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{7C801207-5395-41CC-B54D-9663C1FE511F}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1174,8 +1160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A15366B-D48F-44CE-A8EE-B3457EA299D7}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1190,7 +1176,7 @@
     <col min="9" max="9" width="61.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>47</v>
@@ -1226,8 +1212,8 @@
       <c r="B2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>73</v>
+      <c r="C2" t="s">
+        <v>72</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
@@ -1243,8 +1229,8 @@
       <c r="B3" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>73</v>
+      <c r="C3" t="s">
+        <v>72</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="9"/>
@@ -1253,15 +1239,15 @@
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
     </row>
-    <row r="4" spans="1:9" ht="181.5">
+    <row r="4" spans="1:9" ht="264">
       <c r="A4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="9"/>
@@ -1270,15 +1256,15 @@
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="1:9" ht="409.5">
+    <row r="5" spans="1:9" ht="396">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>76</v>
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>58</v>
@@ -1296,8 +1282,8 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>77</v>
+      <c r="C6" t="s">
+        <v>76</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="9"/>
@@ -1313,8 +1299,8 @@
       <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>77</v>
+      <c r="C7" t="s">
+        <v>76</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="9"/>
@@ -1328,10 +1314,10 @@
         <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>76</v>
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>75</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="9"/>
@@ -1342,13 +1328,13 @@
     </row>
     <row r="9" spans="1:9" ht="409.5">
       <c r="A9" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>74</v>
+      <c r="C9" t="s">
+        <v>73</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="9"/>
@@ -1364,8 +1350,8 @@
       <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>78</v>
+      <c r="C10" t="s">
+        <v>77</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="9"/>
@@ -1381,8 +1367,8 @@
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>76</v>
+      <c r="C11" t="s">
+        <v>75</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="9"/>
@@ -1396,10 +1382,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>78</v>
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>77</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="5" t="s">
@@ -1421,10 +1407,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>78</v>
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="6" t="s">
@@ -1443,15 +1429,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="409.5">
+    <row r="14" spans="1:9" ht="379.5">
       <c r="A14" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="6" t="s">
@@ -1471,10 +1457,10 @@
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>77</v>
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>76</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>20</v>
@@ -1494,8 +1480,8 @@
       <c r="B16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>77</v>
+      <c r="C16" t="s">
+        <v>76</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="9"/>
@@ -1515,10 +1501,10 @@
         <v>23</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>76</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="5" t="s">
@@ -1538,10 +1524,10 @@
         <v>24</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>76</v>
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>75</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="6" t="s">
@@ -1559,10 +1545,10 @@
         <v>45</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>75</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="5" t="s">
@@ -1588,8 +1574,8 @@
       <c r="B20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>73</v>
+      <c r="C20" t="s">
+        <v>72</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="5"/>
@@ -1603,10 +1589,10 @@
         <v>53</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="5"/>
@@ -1622,8 +1608,8 @@
       <c r="B22" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>74</v>
+      <c r="C22" t="s">
+        <v>73</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="5"/>

</xml_diff>